<commit_message>
Denmark data update and barchart
</commit_message>
<xml_diff>
--- a/Data Processing/raw_data/Denmark AMR data organizer JR - March 5 update.xlsx
+++ b/Data Processing/raw_data/Denmark AMR data organizer JR - March 5 update.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\First Analytics\Clients\University of Liverpool\2023-11 Antimicrobial Usage Revisit\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0BC32E5-A74E-4ED8-8B49-0CA20282054F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DC58A05-7DB7-47D0-9E00-816E25E09C22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{AC3DE23B-CCA8-4C55-A652-BAD7C0A905D8}"/>
+    <workbookView xWindow="-3270" yWindow="11920" windowWidth="25760" windowHeight="15440" activeTab="1" xr2:uid="{AC3DE23B-CCA8-4C55-A652-BAD7C0A905D8}"/>
   </bookViews>
   <sheets>
     <sheet name="Farm summary" sheetId="1" r:id="rId1"/>
@@ -172,7 +172,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Health expenditure is not dependent on AMR scenario. NOTE Joao's spreadsheet shows these as positive numbers. I have made them negative to match the production losses.
+Health expenditure is not dependent on AMR scenario. NOTE Joao's spreadsheet shows these as positive numbers. I have made them negative and reversed the 5% and 95% levels to match the production losses.
 </t>
         </r>
       </text>
@@ -738,7 +738,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -748,12 +748,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -810,7 +804,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -825,7 +819,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="168" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
@@ -1216,7 +1209,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1327,8 +1320,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{066FDB34-4E0C-4994-97D4-A599EB20ADE2}">
   <dimension ref="A1:O14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1531,29 +1524,29 @@
         <v>-544280442.82804191</v>
       </c>
       <c r="I6" s="12">
-        <f t="shared" si="4"/>
+        <f>SUM(I3:I5)</f>
         <v>180740669.45309848</v>
       </c>
-      <c r="J6" s="13">
+      <c r="J6" s="12">
         <v>-30732654.23</v>
       </c>
-      <c r="K6" s="13">
+      <c r="K6" s="12">
+        <v>-79746577.519999996</v>
+      </c>
+      <c r="L6" s="12">
         <v>-7686729.46</v>
-      </c>
-      <c r="L6" s="13">
-        <v>-79746577.519999996</v>
       </c>
       <c r="M6" s="12">
         <f>G6+J6</f>
         <v>-211948395.99388185</v>
       </c>
       <c r="N6" s="12">
-        <f t="shared" ref="N6:O6" si="5">H6+K6</f>
-        <v>-551967172.28804195</v>
+        <f>H6+K6</f>
+        <v>-624027020.34804189</v>
       </c>
       <c r="O6" s="12">
-        <f t="shared" si="5"/>
-        <v>100994091.93309848</v>
+        <f>I6+L6</f>
+        <v>173053939.99309847</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -1588,7 +1581,9 @@
         <f t="shared" si="2"/>
         <v>275791358.80396003</v>
       </c>
-      <c r="L7" s="4"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -1622,7 +1617,9 @@
         <f t="shared" si="2"/>
         <v>-276597890.4723056</v>
       </c>
-      <c r="L8" s="4"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -1656,7 +1653,9 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L9" s="4"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
     </row>
     <row r="10" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
@@ -1677,33 +1676,33 @@
         <v>-363602970.34519398</v>
       </c>
       <c r="H10" s="12">
-        <f t="shared" ref="H10:I10" si="6">SUM(H7:H9)</f>
+        <f t="shared" ref="H10:I10" si="5">SUM(H7:H9)</f>
         <v>-728575034.28226256</v>
       </c>
       <c r="I10" s="12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>-806531.66834557056</v>
       </c>
-      <c r="J10" s="13">
+      <c r="J10" s="12">
         <v>-30732654.23</v>
       </c>
-      <c r="K10" s="13">
+      <c r="K10" s="12">
+        <v>-79746577.519999996</v>
+      </c>
+      <c r="L10" s="12">
         <v>-7686729.46</v>
-      </c>
-      <c r="L10" s="13">
-        <v>-79746577.519999996</v>
       </c>
       <c r="M10" s="12">
         <f>G10+J10</f>
         <v>-394335624.575194</v>
       </c>
       <c r="N10" s="12">
-        <f t="shared" ref="N10:O10" si="7">H10+K10</f>
-        <v>-736261763.7422626</v>
+        <f t="shared" ref="N7:N14" si="6">H10+K10</f>
+        <v>-808321611.80226254</v>
       </c>
       <c r="O10" s="12">
-        <f t="shared" si="7"/>
-        <v>-80553109.188345566</v>
+        <f t="shared" ref="O7:O14" si="7">I10+L10</f>
+        <v>-8493261.1283455715</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
@@ -1738,6 +1737,9 @@
         <f t="shared" si="8"/>
         <v>316263789.38339704</v>
       </c>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -1771,6 +1773,9 @@
         <f t="shared" ref="I12:I13" si="11">F12*$C12</f>
         <v>-14223877.023297263</v>
       </c>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -1804,6 +1809,9 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
     </row>
     <row r="14" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
@@ -1831,26 +1839,26 @@
         <f t="shared" si="12"/>
         <v>302039912.36009979</v>
       </c>
-      <c r="J14" s="13">
+      <c r="J14" s="12">
         <v>-30732654.23</v>
       </c>
-      <c r="K14" s="13">
+      <c r="K14" s="12">
+        <v>-79746577.519999996</v>
+      </c>
+      <c r="L14" s="12">
         <v>-7686729.46</v>
-      </c>
-      <c r="L14" s="13">
-        <v>-79746577.519999996</v>
       </c>
       <c r="M14" s="12">
         <f>G14+J14</f>
         <v>-87165678.557697639</v>
       </c>
       <c r="N14" s="12">
-        <f t="shared" ref="N14:O14" si="13">H14+K14</f>
-        <v>-427851368.10476559</v>
+        <f t="shared" si="6"/>
+        <v>-499911216.1647656</v>
       </c>
       <c r="O14" s="12">
-        <f t="shared" si="13"/>
-        <v>222293334.84009981</v>
+        <f t="shared" si="7"/>
+        <v>294353182.90009981</v>
       </c>
     </row>
   </sheetData>
@@ -1874,7 +1882,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1991,13 +1999,13 @@
         <f>SUM(B2:B4)</f>
         <v>2978.1266452200512</v>
       </c>
-      <c r="F5" s="14">
+      <c r="F5" s="13">
         <v>7761284413.2337246</v>
       </c>
-      <c r="G5" s="14">
+      <c r="G5" s="13">
         <v>8353430843.0332108</v>
       </c>
-      <c r="H5" s="14">
+      <c r="H5" s="13">
         <v>7175630833.8693714</v>
       </c>
     </row>
@@ -2061,13 +2069,13 @@
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="4"/>
-      <c r="D2" s="16">
+      <c r="D2" s="15">
         <v>4147189637.4599733</v>
       </c>
-      <c r="E2" s="16">
+      <c r="E2" s="15">
         <v>3799746438.7317729</v>
       </c>
-      <c r="F2" s="15">
+      <c r="F2" s="14">
         <v>4499456508.7119274</v>
       </c>
     </row>
@@ -2077,13 +2085,13 @@
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="4"/>
-      <c r="D3" s="16">
+      <c r="D3" s="15">
         <v>1381511615.1715894</v>
       </c>
-      <c r="E3" s="16">
+      <c r="E3" s="15">
         <v>1315019812.7095423</v>
       </c>
-      <c r="F3" s="15">
+      <c r="F3" s="14">
         <v>1447171527.8463204</v>
       </c>
     </row>
@@ -2093,13 +2101,13 @@
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="4"/>
-      <c r="D4" s="16">
+      <c r="D4" s="15">
         <v>2232583160.6021614</v>
       </c>
-      <c r="E4" s="16">
+      <c r="E4" s="15">
         <v>2060864582.428057</v>
       </c>
-      <c r="F4" s="16">
+      <c r="F4" s="15">
         <v>2406802806.4749675</v>
       </c>
     </row>

</xml_diff>